<commit_message>
Added inflation to rent, corrected the sensitivity plots
</commit_message>
<xml_diff>
--- a/real_estate_roi/Calculs.xlsx
+++ b/real_estate_roi/Calculs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ronan\code\Invest\real_estate_roi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F7AC91-0E4E-40FC-A5ED-CEB43BD97708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D22A95-6F25-47D8-9737-DD8CD7B70095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{82EA677A-568B-47B4-8E28-A278992804B1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>year</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Frais de vente</t>
+  </si>
+  <si>
+    <t>Inflation</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="A2:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -595,6 +598,14 @@
         <v>800</v>
       </c>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.02</v>
+      </c>
+    </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>0</v>
@@ -663,7 +674,7 @@
         <v>52500</v>
       </c>
       <c r="C9" s="12">
-        <f>C8+$C$3*12</f>
+        <f>C8+($C$3*(1+$C$4)^($A9-1))*12</f>
         <v>9600</v>
       </c>
       <c r="D9" s="12">
@@ -696,12 +707,12 @@
         <v>55125</v>
       </c>
       <c r="C10" s="12">
-        <f t="shared" ref="C10:C18" si="2">C9+$C$3*12</f>
-        <v>19200</v>
+        <f t="shared" ref="C10:C18" si="2">C9+($C$3*(1+$C$4)^($A10-1))*12</f>
+        <v>19392</v>
       </c>
       <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>35925</v>
+        <v>35733</v>
       </c>
       <c r="I10" s="2">
         <v>2</v>
@@ -710,10 +721,10 @@
         <v>55125</v>
       </c>
       <c r="K10" s="2">
-        <v>19200</v>
+        <v>19392</v>
       </c>
       <c r="L10" s="2">
-        <v>35925</v>
+        <v>35733</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -730,11 +741,11 @@
       </c>
       <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>28800</v>
+        <v>29379.84</v>
       </c>
       <c r="D11" s="12">
         <f t="shared" si="0"/>
-        <v>29081.25</v>
+        <v>28501.41</v>
       </c>
       <c r="I11" s="2">
         <v>3</v>
@@ -743,10 +754,10 @@
         <v>57881.25</v>
       </c>
       <c r="K11" s="2">
-        <v>28800</v>
+        <v>29379.84</v>
       </c>
       <c r="L11" s="2">
-        <v>29081.25</v>
+        <v>28501.41</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -763,11 +774,11 @@
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>38400</v>
+        <v>39567.436799999996</v>
       </c>
       <c r="D12" s="12">
         <f t="shared" si="0"/>
-        <v>22375.3125</v>
+        <v>21207.875700000004</v>
       </c>
       <c r="I12" s="2">
         <v>4</v>
@@ -776,10 +787,10 @@
         <v>60775.3125</v>
       </c>
       <c r="K12" s="2">
-        <v>38400</v>
+        <v>39567.436800000003</v>
       </c>
       <c r="L12" s="2">
-        <v>22375.3125</v>
+        <v>21207.875700000001</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -796,11 +807,11 @@
       </c>
       <c r="C13" s="12">
         <f t="shared" si="2"/>
-        <v>48000</v>
+        <v>49958.785535999996</v>
       </c>
       <c r="D13" s="12">
         <f t="shared" si="0"/>
-        <v>15814.078125</v>
+        <v>13855.292589000004</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -809,10 +820,10 @@
         <v>63814.078125</v>
       </c>
       <c r="K13" s="2">
-        <v>48000</v>
+        <v>49958.785536000003</v>
       </c>
       <c r="L13" s="2">
-        <v>15814.078125</v>
+        <v>13855.292589000001</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -829,11 +840,11 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>57600</v>
+        <v>60557.961246719991</v>
       </c>
       <c r="D14" s="12">
         <f t="shared" si="0"/>
-        <v>9404.7820312499971</v>
+        <v>6446.8207845300058</v>
       </c>
       <c r="I14" s="2">
         <v>6</v>
@@ -842,10 +853,10 @@
         <v>67004.782031249997</v>
       </c>
       <c r="K14" s="2">
-        <v>57600</v>
+        <v>60557.961246719999</v>
       </c>
       <c r="L14" s="2">
-        <v>9404.7820312500207</v>
+        <v>6446.8207845300203</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -862,11 +873,11 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>67200</v>
+        <v>71369.120471654387</v>
       </c>
       <c r="D15" s="12">
         <f t="shared" si="0"/>
-        <v>3155.0211328125006</v>
+        <v>-1014.0993388418865</v>
       </c>
       <c r="I15" s="2">
         <v>7</v>
@@ -875,10 +886,10 @@
         <v>70355.021132812501</v>
       </c>
       <c r="K15" s="2">
-        <v>67200</v>
+        <v>71369.120471654402</v>
       </c>
       <c r="L15" s="2">
-        <v>3155.0211328125201</v>
+        <v>-1014.09933884187</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -895,11 +906,11 @@
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>76800</v>
+        <v>82396.502881087479</v>
       </c>
       <c r="D16" s="12">
         <f t="shared" si="0"/>
-        <v>-2927.2278105468722</v>
+        <v>-8523.7306916343514</v>
       </c>
       <c r="I16" s="2">
         <v>8</v>
@@ -908,10 +919,10 @@
         <v>73872.772189453099</v>
       </c>
       <c r="K16" s="2">
-        <v>76800</v>
+        <v>82396.502881087494</v>
       </c>
       <c r="L16" s="2">
-        <v>-2927.2278105468399</v>
+        <v>-8523.7306916343296</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -928,11 +939,11 @@
       </c>
       <c r="C17" s="12">
         <f t="shared" si="2"/>
-        <v>86400</v>
+        <v>93644.432938709229</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" si="0"/>
-        <v>-8833.58920107421</v>
+        <v>-16078.022139783439</v>
       </c>
       <c r="I17" s="2">
         <v>9</v>
@@ -941,10 +952,10 @@
         <v>77566.410798925805</v>
       </c>
       <c r="K17" s="2">
-        <v>86400</v>
+        <v>93644.4329387092</v>
       </c>
       <c r="L17" s="2">
-        <v>-8833.58920107419</v>
+        <v>-16078.022139783399</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
@@ -957,11 +968,11 @@
       </c>
       <c r="C18" s="12">
         <f t="shared" si="2"/>
-        <v>96000</v>
+        <v>105117.32159748342</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="0"/>
-        <v>-14555.26866112792</v>
+        <v>-23672.590258611337</v>
       </c>
       <c r="I18" s="2">
         <v>10</v>
@@ -970,10 +981,10 @@
         <v>81444.731338872094</v>
       </c>
       <c r="K18" s="2">
-        <v>96000</v>
+        <v>105117.32159748299</v>
       </c>
       <c r="L18" s="2">
-        <v>-14555.2686611279</v>
+        <v>-23672.590258611301</v>
       </c>
     </row>
   </sheetData>
@@ -985,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5909263E-C9E0-4C5D-A11C-FB7D5DCDA3C7}">
   <dimension ref="B2:T60"/>
   <sheetViews>
-    <sheetView topLeftCell="C27" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2032,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B38-1)+$F$35*G38/12)</f>
+        <f t="shared" ref="D38:D54" si="3">-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B38-1)+$F$35*G38/12)</f>
         <v>-457.96875</v>
       </c>
       <c r="E38" s="13">
@@ -2086,11 +2097,11 @@
         <v>2</v>
       </c>
       <c r="D39" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B39-1)+$F$35*G39/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E39" s="13">
-        <f t="shared" ref="E39:E54" si="3">D39-D11</f>
+        <f t="shared" ref="E39:E54" si="4">D39-D11</f>
         <v>-1715.54002200943</v>
       </c>
       <c r="F39" s="13">
@@ -2102,11 +2113,11 @@
         <v>250000</v>
       </c>
       <c r="H39" s="11">
-        <f t="shared" ref="H39:H54" si="4">G11</f>
+        <f t="shared" ref="H39:H54" si="5">G11</f>
         <v>237321.64610729666</v>
       </c>
       <c r="I39" s="11">
-        <f t="shared" ref="I39:I54" si="5">G39-H39+F39</f>
+        <f t="shared" ref="I39:I53" si="6">G39-H39+F39</f>
         <v>-40752.726151315524</v>
       </c>
       <c r="J39" s="3"/>
@@ -2140,27 +2151,27 @@
         <v>3</v>
       </c>
       <c r="D40" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B40-1)+$F$35*G40/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E40" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F40" s="13">
-        <f t="shared" ref="F40:F54" si="6">F39+E40</f>
+        <f t="shared" ref="F40:F54" si="7">F39+E40</f>
         <v>-55146.620066028292</v>
       </c>
       <c r="G40" s="14">
-        <f t="shared" ref="G40:G54" si="7">G39*(1+$I$33/12)</f>
+        <f t="shared" ref="G40:G54" si="8">G39*(1+$I$33/12)</f>
         <v>250000</v>
       </c>
       <c r="H40" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>236855.14698897823</v>
       </c>
       <c r="I40" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-42001.767055006523</v>
       </c>
       <c r="J40" s="3"/>
@@ -2194,27 +2205,27 @@
         <v>4</v>
       </c>
       <c r="D41" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B41-1)+$F$35*G41/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E41" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F41" s="13">
+        <f t="shared" si="7"/>
+        <v>-56862.160088037723</v>
+      </c>
+      <c r="G41" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H41" s="11">
+        <f t="shared" si="5"/>
+        <v>236387.09287359874</v>
+      </c>
+      <c r="I41" s="11">
         <f t="shared" si="6"/>
-        <v>-56862.160088037723</v>
-      </c>
-      <c r="G41" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H41" s="11">
-        <f t="shared" si="4"/>
-        <v>236387.09287359874</v>
-      </c>
-      <c r="I41" s="11">
-        <f t="shared" si="5"/>
         <v>-43249.252961636463</v>
       </c>
       <c r="J41" s="3"/>
@@ -2248,27 +2259,27 @@
         <v>5</v>
       </c>
       <c r="D42" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B42-1)+$F$35*G42/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E42" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F42" s="13">
+        <f t="shared" si="7"/>
+        <v>-58577.700110047153</v>
+      </c>
+      <c r="G42" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H42" s="11">
+        <f t="shared" si="5"/>
+        <v>235917.47857783464</v>
+      </c>
+      <c r="I42" s="11">
         <f t="shared" si="6"/>
-        <v>-58577.700110047153</v>
-      </c>
-      <c r="G42" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H42" s="11">
-        <f t="shared" si="4"/>
-        <v>235917.47857783464</v>
-      </c>
-      <c r="I42" s="11">
-        <f t="shared" si="5"/>
         <v>-44495.178687881795</v>
       </c>
       <c r="J42" s="3"/>
@@ -2302,27 +2313,27 @@
         <v>6</v>
       </c>
       <c r="D43" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B43-1)+$F$35*G43/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E43" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F43" s="13">
+        <f t="shared" si="7"/>
+        <v>-60293.240132056584</v>
+      </c>
+      <c r="G43" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H43" s="11">
+        <f t="shared" si="5"/>
+        <v>235446.29890108466</v>
+      </c>
+      <c r="I43" s="11">
         <f t="shared" si="6"/>
-        <v>-60293.240132056584</v>
-      </c>
-      <c r="G43" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H43" s="11">
-        <f t="shared" si="4"/>
-        <v>235446.29890108466</v>
-      </c>
-      <c r="I43" s="11">
-        <f t="shared" si="5"/>
         <v>-45739.539033141249</v>
       </c>
       <c r="J43" s="3"/>
@@ -2356,27 +2367,27 @@
         <v>7</v>
       </c>
       <c r="D44" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B44-1)+$F$35*G44/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E44" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F44" s="13">
+        <f t="shared" si="7"/>
+        <v>-62008.780154066015</v>
+      </c>
+      <c r="G44" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H44" s="11">
+        <f t="shared" si="5"/>
+        <v>234973.54862541219</v>
+      </c>
+      <c r="I44" s="11">
         <f t="shared" si="6"/>
-        <v>-62008.780154066015</v>
-      </c>
-      <c r="G44" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H44" s="11">
-        <f t="shared" si="4"/>
-        <v>234973.54862541219</v>
-      </c>
-      <c r="I44" s="11">
-        <f t="shared" si="5"/>
         <v>-46982.328779478208</v>
       </c>
       <c r="J44" s="3"/>
@@ -2410,27 +2421,27 @@
         <v>8</v>
       </c>
       <c r="D45" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B45-1)+$F$35*G45/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E45" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F45" s="13">
+        <f t="shared" si="7"/>
+        <v>-63724.320176075445</v>
+      </c>
+      <c r="G45" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H45" s="11">
+        <f t="shared" si="5"/>
+        <v>234499.22251548746</v>
+      </c>
+      <c r="I45" s="11">
         <f t="shared" si="6"/>
-        <v>-63724.320176075445</v>
-      </c>
-      <c r="G45" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H45" s="11">
-        <f t="shared" si="4"/>
-        <v>234499.22251548746</v>
-      </c>
-      <c r="I45" s="11">
-        <f t="shared" si="5"/>
         <v>-48223.542691562907</v>
       </c>
       <c r="J45" s="3"/>
@@ -2464,27 +2475,27 @@
         <v>9</v>
       </c>
       <c r="D46" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B46-1)+$F$35*G46/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E46" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F46" s="13">
+        <f t="shared" si="7"/>
+        <v>-65439.860198084876</v>
+      </c>
+      <c r="G46" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H46" s="11">
+        <f t="shared" si="5"/>
+        <v>234023.31531852967</v>
+      </c>
+      <c r="I46" s="11">
         <f t="shared" si="6"/>
-        <v>-65439.860198084876</v>
-      </c>
-      <c r="G46" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H46" s="11">
-        <f t="shared" si="4"/>
-        <v>234023.31531852967</v>
-      </c>
-      <c r="I46" s="11">
-        <f t="shared" si="5"/>
         <v>-49463.175516614545</v>
       </c>
       <c r="J46" s="3"/>
@@ -2518,27 +2529,27 @@
         <v>10</v>
       </c>
       <c r="D47" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B47-1)+$F$35*G47/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E47" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F47" s="13">
+        <f t="shared" si="7"/>
+        <v>-67155.400220094307</v>
+      </c>
+      <c r="G47" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H47" s="11">
+        <f t="shared" si="5"/>
+        <v>233545.82176424869</v>
+      </c>
+      <c r="I47" s="11">
         <f t="shared" si="6"/>
-        <v>-67155.400220094307</v>
-      </c>
-      <c r="G47" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H47" s="11">
-        <f t="shared" si="4"/>
-        <v>233545.82176424869</v>
-      </c>
-      <c r="I47" s="11">
-        <f t="shared" si="5"/>
         <v>-50701.221984342992</v>
       </c>
       <c r="J47" s="3"/>
@@ -2572,27 +2583,27 @@
         <v>11</v>
       </c>
       <c r="D48" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B48-1)+$F$35*G48/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E48" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F48" s="13">
+        <f t="shared" si="7"/>
+        <v>-68870.940242103738</v>
+      </c>
+      <c r="G48" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H48" s="11">
+        <f t="shared" si="5"/>
+        <v>233066.73656478676</v>
+      </c>
+      <c r="I48" s="11">
         <f t="shared" si="6"/>
-        <v>-68870.940242103738</v>
-      </c>
-      <c r="G48" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H48" s="11">
-        <f t="shared" si="4"/>
-        <v>233066.73656478676</v>
-      </c>
-      <c r="I48" s="11">
-        <f t="shared" si="5"/>
         <v>-51937.676806890493</v>
       </c>
       <c r="J48" s="3"/>
@@ -2626,27 +2637,27 @@
         <v>12</v>
       </c>
       <c r="D49" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B49-1)+$F$35*G49/12)</f>
+        <f t="shared" si="3"/>
         <v>-457.96875</v>
       </c>
       <c r="E49" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1715.54002200943</v>
       </c>
       <c r="F49" s="13">
+        <f t="shared" si="7"/>
+        <v>-70586.480264113168</v>
+      </c>
+      <c r="G49" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="5"/>
+        <v>232586.05441465994</v>
+      </c>
+      <c r="I49" s="11">
         <f t="shared" si="6"/>
-        <v>-70586.480264113168</v>
-      </c>
-      <c r="G49" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H49" s="11">
-        <f t="shared" si="4"/>
-        <v>232586.05441465994</v>
-      </c>
-      <c r="I49" s="11">
-        <f t="shared" si="5"/>
         <v>-53172.53467877311</v>
       </c>
       <c r="J49" s="3"/>
@@ -2680,27 +2691,27 @@
         <v>1</v>
       </c>
       <c r="D50" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B50-1)+$F$35*G50/12)</f>
+        <f t="shared" si="3"/>
         <v>-459.96875</v>
       </c>
       <c r="E50" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1717.54002200943</v>
       </c>
       <c r="F50" s="13">
+        <f t="shared" si="7"/>
+        <v>-72304.020286122599</v>
+      </c>
+      <c r="G50" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H50" s="11">
+        <f t="shared" si="5"/>
+        <v>232103.76999069937</v>
+      </c>
+      <c r="I50" s="11">
         <f t="shared" si="6"/>
-        <v>-72304.020286122599</v>
-      </c>
-      <c r="G50" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H50" s="11">
-        <f t="shared" si="4"/>
-        <v>232103.76999069937</v>
-      </c>
-      <c r="I50" s="11">
-        <f t="shared" si="5"/>
         <v>-54407.790276821965</v>
       </c>
       <c r="J50" s="3"/>
@@ -2734,27 +2745,27 @@
         <v>2</v>
       </c>
       <c r="D51" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B51-1)+$F$35*G51/12)</f>
+        <f t="shared" si="3"/>
         <v>-459.96875</v>
       </c>
       <c r="E51" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1717.54002200943</v>
       </c>
       <c r="F51" s="13">
+        <f t="shared" si="7"/>
+        <v>-74021.56030813203</v>
+      </c>
+      <c r="G51" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H51" s="11">
+        <f t="shared" si="5"/>
+        <v>231619.87795199227</v>
+      </c>
+      <c r="I51" s="11">
         <f t="shared" si="6"/>
-        <v>-74021.56030813203</v>
-      </c>
-      <c r="G51" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H51" s="11">
-        <f t="shared" si="4"/>
-        <v>231619.87795199227</v>
-      </c>
-      <c r="I51" s="11">
-        <f t="shared" si="5"/>
         <v>-55641.438260124298</v>
       </c>
       <c r="J51" s="3"/>
@@ -2788,27 +2799,27 @@
         <v>3</v>
       </c>
       <c r="D52" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B52-1)+$F$35*G52/12)</f>
+        <f t="shared" si="3"/>
         <v>-459.96875</v>
       </c>
       <c r="E52" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1717.54002200943</v>
       </c>
       <c r="F52" s="13">
+        <f t="shared" si="7"/>
+        <v>-75739.10033014146</v>
+      </c>
+      <c r="G52" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H52" s="11">
+        <f t="shared" si="5"/>
+        <v>231134.37293982282</v>
+      </c>
+      <c r="I52" s="11">
         <f t="shared" si="6"/>
-        <v>-75739.10033014146</v>
-      </c>
-      <c r="G52" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H52" s="11">
-        <f t="shared" si="4"/>
-        <v>231134.37293982282</v>
-      </c>
-      <c r="I52" s="11">
-        <f t="shared" si="5"/>
         <v>-56873.473269964277</v>
       </c>
       <c r="J52" s="3"/>
@@ -2842,27 +2853,27 @@
         <v>4</v>
       </c>
       <c r="D53" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B53-1)+$F$35*G53/12)</f>
+        <f t="shared" si="3"/>
         <v>-459.96875</v>
       </c>
       <c r="E53" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1717.54002200943</v>
       </c>
       <c r="F53" s="13">
+        <f t="shared" si="7"/>
+        <v>-77456.640352150891</v>
+      </c>
+      <c r="G53" s="14">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H53" s="11">
+        <f t="shared" si="5"/>
+        <v>230647.24957761279</v>
+      </c>
+      <c r="I53" s="11">
         <f t="shared" si="6"/>
-        <v>-77456.640352150891</v>
-      </c>
-      <c r="G53" s="14">
-        <f t="shared" si="7"/>
-        <v>250000</v>
-      </c>
-      <c r="H53" s="11">
-        <f t="shared" si="4"/>
-        <v>230647.24957761279</v>
-      </c>
-      <c r="I53" s="11">
-        <f t="shared" si="5"/>
         <v>-58103.889929763682</v>
       </c>
       <c r="J53" s="3"/>
@@ -2896,23 +2907,23 @@
         <v>5</v>
       </c>
       <c r="D54" s="12">
-        <f>-($C$33/12+$C$35*$G$3/12+$F$33/12*(1+$F$34)^($B54-1)+$F$35*G54/12)</f>
+        <f t="shared" si="3"/>
         <v>-459.96875</v>
       </c>
       <c r="E54" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1717.54002200943</v>
       </c>
       <c r="F54" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-79174.180374160322</v>
       </c>
       <c r="G54" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>250000</v>
       </c>
       <c r="H54" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>230158.50247086206</v>
       </c>
       <c r="I54" s="11">
@@ -2977,7 +2988,7 @@
         <v>65751.188366737348</v>
       </c>
       <c r="Q59" s="11">
-        <f t="shared" ref="Q59" si="8">Q58+P59</f>
+        <f t="shared" ref="Q59" si="9">Q58+P59</f>
         <v>-189518.23019520863</v>
       </c>
       <c r="R59" s="2">

</xml_diff>